<commit_message>
code and schema refactored
</commit_message>
<xml_diff>
--- a/prisma/seed/data/cheapblinds_data.xlsx
+++ b/prisma/seed/data/cheapblinds_data.xlsx
@@ -1201,10 +1201,10 @@
         <v>Blackout Roller Blinds</v>
       </c>
       <c r="C2" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D2" t="str">
-        <v>e6b109b1-def8-4676-b34b-0605cc072c45</v>
+        <v>fd858631-07a9-44f8-ab72-46928d93d15f</v>
       </c>
       <c r="E2" t="str">
         <v>Classic Roller Blind</v>
@@ -1290,10 +1290,10 @@
         <v>Blackout Roller Blinds</v>
       </c>
       <c r="C3" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D3" t="str">
-        <v>e6b109b1-def8-4676-b34b-0605cc072c45</v>
+        <v>fd858631-07a9-44f8-ab72-46928d93d15f</v>
       </c>
       <c r="E3" t="str">
         <v>Wooden Venetian Blind</v>
@@ -1379,10 +1379,10 @@
         <v>Blackout Roller Blinds</v>
       </c>
       <c r="C4" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D4" t="str">
-        <v>e6b109b1-def8-4676-b34b-0605cc072c45</v>
+        <v>fd858631-07a9-44f8-ab72-46928d93d15f</v>
       </c>
       <c r="E4" t="str">
         <v>Blackout Shade</v>
@@ -1468,10 +1468,10 @@
         <v>Blackout Roller Blinds</v>
       </c>
       <c r="C5" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D5" t="str">
-        <v>e6b109b1-def8-4676-b34b-0605cc072c45</v>
+        <v>fd858631-07a9-44f8-ab72-46928d93d15f</v>
       </c>
       <c r="E5" t="str">
         <v>Sheer Curtain</v>
@@ -1557,10 +1557,10 @@
         <v>See-through Roller Blind</v>
       </c>
       <c r="C6" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D6" t="str">
-        <v>bf131059-09a8-4ecd-b005-5ff45bad3e96</v>
+        <v>dad2b61c-dcdc-460a-86a2-4b78aad14146</v>
       </c>
       <c r="E6" t="str">
         <v>Blackout Curtain</v>
@@ -1646,10 +1646,10 @@
         <v>See-through Roller Blind</v>
       </c>
       <c r="C7" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D7" t="str">
-        <v>bf131059-09a8-4ecd-b005-5ff45bad3e96</v>
+        <v>dad2b61c-dcdc-460a-86a2-4b78aad14146</v>
       </c>
       <c r="E7" t="str">
         <v>Decorative Valance</v>
@@ -1735,10 +1735,10 @@
         <v>See-through Roller Blind</v>
       </c>
       <c r="C8" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D8" t="str">
-        <v>bf131059-09a8-4ecd-b005-5ff45bad3e96</v>
+        <v>dad2b61c-dcdc-460a-86a2-4b78aad14146</v>
       </c>
       <c r="E8" t="str">
         <v>Mounting Brackets</v>
@@ -1824,10 +1824,10 @@
         <v>See-through Roller Blind</v>
       </c>
       <c r="C9" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D9" t="str">
-        <v>bf131059-09a8-4ecd-b005-5ff45bad3e96</v>
+        <v>dad2b61c-dcdc-460a-86a2-4b78aad14146</v>
       </c>
       <c r="E9" t="str">
         <v>Panel Blind</v>
@@ -1913,10 +1913,10 @@
         <v>See-through Roller Blind</v>
       </c>
       <c r="C10" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D10" t="str">
-        <v>bf131059-09a8-4ecd-b005-5ff45bad3e96</v>
+        <v>dad2b61c-dcdc-460a-86a2-4b78aad14146</v>
       </c>
       <c r="E10" t="str">
         <v>Cellular Shade</v>
@@ -2002,10 +2002,10 @@
         <v>Dimout Roller Blinds</v>
       </c>
       <c r="C11" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D11" t="str">
-        <v>1201ed01-fc66-4b41-a720-825a63b7d326</v>
+        <v>e96b16a1-1db4-4fdb-9227-f63d14771655</v>
       </c>
       <c r="E11" t="str">
         <v>Motorized Roller Blind</v>
@@ -2091,10 +2091,10 @@
         <v>Dimout Roller Blinds</v>
       </c>
       <c r="C12" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D12" t="str">
-        <v>1201ed01-fc66-4b41-a720-825a63b7d326</v>
+        <v>e96b16a1-1db4-4fdb-9227-f63d14771655</v>
       </c>
       <c r="E12" t="str">
         <v>Premium Roller Blind</v>
@@ -2180,10 +2180,10 @@
         <v>Dimout Roller Blinds</v>
       </c>
       <c r="C13" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D13" t="str">
-        <v>1201ed01-fc66-4b41-a720-825a63b7d326</v>
+        <v>e96b16a1-1db4-4fdb-9227-f63d14771655</v>
       </c>
       <c r="E13" t="str">
         <v>Dual Layer Roller Blind</v>
@@ -2269,10 +2269,10 @@
         <v>Waterproof Roller Blinds</v>
       </c>
       <c r="C14" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D14" t="str">
-        <v>62fd2b87-f836-4949-b5a4-53739e6ca069</v>
+        <v>a8c771b0-910e-4b5b-bc0c-1902d4476642</v>
       </c>
       <c r="E14" t="str">
         <v>Day Night Roller Blind</v>
@@ -2358,10 +2358,10 @@
         <v>Waterproof Roller Blinds</v>
       </c>
       <c r="C15" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D15" t="str">
-        <v>62fd2b87-f836-4949-b5a4-53739e6ca069</v>
+        <v>a8c771b0-910e-4b5b-bc0c-1902d4476642</v>
       </c>
       <c r="E15" t="str">
         <v>PVC Venetian Blind</v>
@@ -2447,10 +2447,10 @@
         <v>Waterproof Roller Blinds</v>
       </c>
       <c r="C16" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D16" t="str">
-        <v>62fd2b87-f836-4949-b5a4-53739e6ca069</v>
+        <v>a8c771b0-910e-4b5b-bc0c-1902d4476642</v>
       </c>
       <c r="E16" t="str">
         <v>Aluminum Venetian Blind</v>
@@ -2536,10 +2536,10 @@
         <v>Waterproof Roller Blinds</v>
       </c>
       <c r="C17" t="str">
-        <v>ef348472-613b-444c-999c-094fb8793d0b</v>
+        <v>f20adf46-e21b-4475-bc9c-1c157ef7610d</v>
       </c>
       <c r="D17" t="str">
-        <v>62fd2b87-f836-4949-b5a4-53739e6ca069</v>
+        <v>a8c771b0-910e-4b5b-bc0c-1902d4476642</v>
       </c>
       <c r="E17" t="str">
         <v>Fabric Roman Blind</v>
@@ -2625,10 +2625,10 @@
         <v>Blackout Roman Blinds</v>
       </c>
       <c r="C18" t="str">
-        <v>004af3f7-f2e7-4040-8cf8-1d210f16dbd1</v>
+        <v>2e31f713-54ce-47d9-9a21-a14352ef6901</v>
       </c>
       <c r="D18" t="str">
-        <v>75487737-c412-4663-a606-b6f190271911</v>
+        <v>2d78856f-75a7-49a8-9467-a8e65d9b2eae</v>
       </c>
       <c r="E18" t="str">
         <v>Luxury Roman Blind</v>
@@ -2714,10 +2714,10 @@
         <v>Blackout Roman Blinds</v>
       </c>
       <c r="C19" t="str">
-        <v>004af3f7-f2e7-4040-8cf8-1d210f16dbd1</v>
+        <v>2e31f713-54ce-47d9-9a21-a14352ef6901</v>
       </c>
       <c r="D19" t="str">
-        <v>75487737-c412-4663-a606-b6f190271911</v>
+        <v>2d78856f-75a7-49a8-9467-a8e65d9b2eae</v>
       </c>
       <c r="E19" t="str">
         <v>Thermal Blackout Blind</v>
@@ -2803,10 +2803,10 @@
         <v>Blackout Roman Blinds</v>
       </c>
       <c r="C20" t="str">
-        <v>004af3f7-f2e7-4040-8cf8-1d210f16dbd1</v>
+        <v>2e31f713-54ce-47d9-9a21-a14352ef6901</v>
       </c>
       <c r="D20" t="str">
-        <v>75487737-c412-4663-a606-b6f190271911</v>
+        <v>2d78856f-75a7-49a8-9467-a8e65d9b2eae</v>
       </c>
       <c r="E20" t="str">
         <v>Printed Roller Blind</v>
@@ -2892,10 +2892,10 @@
         <v>Blackout Roman Blinds</v>
       </c>
       <c r="C21" t="str">
-        <v>004af3f7-f2e7-4040-8cf8-1d210f16dbd1</v>
+        <v>2e31f713-54ce-47d9-9a21-a14352ef6901</v>
       </c>
       <c r="D21" t="str">
-        <v>75487737-c412-4663-a606-b6f190271911</v>
+        <v>2d78856f-75a7-49a8-9467-a8e65d9b2eae</v>
       </c>
       <c r="E21" t="str">
         <v>Plain White Roller Blind</v>
@@ -2981,10 +2981,10 @@
         <v>See-through Roman Blinds</v>
       </c>
       <c r="C22" t="str">
-        <v>004af3f7-f2e7-4040-8cf8-1d210f16dbd1</v>
+        <v>2e31f713-54ce-47d9-9a21-a14352ef6901</v>
       </c>
       <c r="D22" t="str">
-        <v>b20d318c-2420-499a-9cf2-0cf5c25a0000</v>
+        <v>0b138f75-7651-4e52-9618-73bd83bddad6</v>
       </c>
       <c r="E22" t="str">
         <v>Smart Motorized Blind</v>
@@ -3070,10 +3070,10 @@
         <v>See-through Roman Blinds</v>
       </c>
       <c r="C23" t="str">
-        <v>004af3f7-f2e7-4040-8cf8-1d210f16dbd1</v>
+        <v>2e31f713-54ce-47d9-9a21-a14352ef6901</v>
       </c>
       <c r="D23" t="str">
-        <v>b20d318c-2420-499a-9cf2-0cf5c25a0000</v>
+        <v>0b138f75-7651-4e52-9618-73bd83bddad6</v>
       </c>
       <c r="E23" t="str">
         <v>Remote Control Blind</v>
@@ -3159,10 +3159,10 @@
         <v>See-through Roman Blinds</v>
       </c>
       <c r="C24" t="str">
-        <v>004af3f7-f2e7-4040-8cf8-1d210f16dbd1</v>
+        <v>2e31f713-54ce-47d9-9a21-a14352ef6901</v>
       </c>
       <c r="D24" t="str">
-        <v>b20d318c-2420-499a-9cf2-0cf5c25a0000</v>
+        <v>0b138f75-7651-4e52-9618-73bd83bddad6</v>
       </c>
       <c r="E24" t="str">
         <v>Cordless Roller Blind</v>
@@ -3248,10 +3248,10 @@
         <v>Dim-out Roman Blinds</v>
       </c>
       <c r="C25" t="str">
-        <v>004af3f7-f2e7-4040-8cf8-1d210f16dbd1</v>
+        <v>2e31f713-54ce-47d9-9a21-a14352ef6901</v>
       </c>
       <c r="D25" t="str">
-        <v>9c33155e-3de9-47e1-8bcc-4f17175b2d9c</v>
+        <v>0a6649da-c760-4c59-a2f2-7ef3f5284103</v>
       </c>
       <c r="E25" t="str">
         <v>Waterproof Roller Blind</v>
@@ -3337,10 +3337,10 @@
         <v>Dim-out Roman Blinds</v>
       </c>
       <c r="C26" t="str">
-        <v>004af3f7-f2e7-4040-8cf8-1d210f16dbd1</v>
+        <v>2e31f713-54ce-47d9-9a21-a14352ef6901</v>
       </c>
       <c r="D26" t="str">
-        <v>9c33155e-3de9-47e1-8bcc-4f17175b2d9c</v>
+        <v>0a6649da-c760-4c59-a2f2-7ef3f5284103</v>
       </c>
       <c r="E26" t="str">
         <v>Kitchen Roller Blind</v>
@@ -3426,10 +3426,10 @@
         <v>Dim-out Roman Blinds</v>
       </c>
       <c r="C27" t="str">
-        <v>004af3f7-f2e7-4040-8cf8-1d210f16dbd1</v>
+        <v>2e31f713-54ce-47d9-9a21-a14352ef6901</v>
       </c>
       <c r="D27" t="str">
-        <v>9c33155e-3de9-47e1-8bcc-4f17175b2d9c</v>
+        <v>0a6649da-c760-4c59-a2f2-7ef3f5284103</v>
       </c>
       <c r="E27" t="str">
         <v>Bathroom Roller Blind</v>
@@ -3515,10 +3515,10 @@
         <v>Dimout Zebra Blind</v>
       </c>
       <c r="C28" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D28" t="str">
-        <v>16d59265-ba58-48d9-a948-36f1f3ea61dd</v>
+        <v>17744f51-bf2e-4def-a6c5-dd29fd9f4a46</v>
       </c>
       <c r="E28" t="str">
         <v>Office Roller Blind</v>
@@ -3604,10 +3604,10 @@
         <v>Dimout Zebra Blind</v>
       </c>
       <c r="C29" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D29" t="str">
-        <v>16d59265-ba58-48d9-a948-36f1f3ea61dd</v>
+        <v>17744f51-bf2e-4def-a6c5-dd29fd9f4a46</v>
       </c>
       <c r="E29" t="str">
         <v>Vertical Blind</v>
@@ -3693,10 +3693,10 @@
         <v>Dimout Zebra Blind</v>
       </c>
       <c r="C30" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D30" t="str">
-        <v>16d59265-ba58-48d9-a948-36f1f3ea61dd</v>
+        <v>17744f51-bf2e-4def-a6c5-dd29fd9f4a46</v>
       </c>
       <c r="E30" t="str">
         <v>Fabric Vertical Blind</v>
@@ -3782,10 +3782,10 @@
         <v>Dimout Zebra Blind</v>
       </c>
       <c r="C31" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D31" t="str">
-        <v>16d59265-ba58-48d9-a948-36f1f3ea61dd</v>
+        <v>17744f51-bf2e-4def-a6c5-dd29fd9f4a46</v>
       </c>
       <c r="E31" t="str">
         <v>PVC Vertical Blind</v>
@@ -3871,10 +3871,10 @@
         <v>Dimout Zebra Blind</v>
       </c>
       <c r="C32" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D32" t="str">
-        <v>16d59265-ba58-48d9-a948-36f1f3ea61dd</v>
+        <v>17744f51-bf2e-4def-a6c5-dd29fd9f4a46</v>
       </c>
       <c r="E32" t="str">
         <v>Classic Curtain Panel</v>
@@ -3960,10 +3960,10 @@
         <v>Dimout Zebra Blind</v>
       </c>
       <c r="C33" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D33" t="str">
-        <v>16d59265-ba58-48d9-a948-36f1f3ea61dd</v>
+        <v>17744f51-bf2e-4def-a6c5-dd29fd9f4a46</v>
       </c>
       <c r="E33" t="str">
         <v>Eyelet Curtain</v>
@@ -4049,10 +4049,10 @@
         <v>Dimout Zebra Blind</v>
       </c>
       <c r="C34" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D34" t="str">
-        <v>16d59265-ba58-48d9-a948-36f1f3ea61dd</v>
+        <v>17744f51-bf2e-4def-a6c5-dd29fd9f4a46</v>
       </c>
       <c r="E34" t="str">
         <v>Pinch Pleat Curtain</v>
@@ -4138,10 +4138,10 @@
         <v>Dimout Zebra Blind</v>
       </c>
       <c r="C35" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D35" t="str">
-        <v>16d59265-ba58-48d9-a948-36f1f3ea61dd</v>
+        <v>17744f51-bf2e-4def-a6c5-dd29fd9f4a46</v>
       </c>
       <c r="E35" t="str">
         <v>Linen Curtain</v>
@@ -4227,10 +4227,10 @@
         <v>Dimout Zebra Blind</v>
       </c>
       <c r="C36" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D36" t="str">
-        <v>16d59265-ba58-48d9-a948-36f1f3ea61dd</v>
+        <v>17744f51-bf2e-4def-a6c5-dd29fd9f4a46</v>
       </c>
       <c r="E36" t="str">
         <v>Velvet Curtain</v>
@@ -4316,10 +4316,10 @@
         <v>Dimout Zebra Blind</v>
       </c>
       <c r="C37" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D37" t="str">
-        <v>16d59265-ba58-48d9-a948-36f1f3ea61dd</v>
+        <v>17744f51-bf2e-4def-a6c5-dd29fd9f4a46</v>
       </c>
       <c r="E37" t="str">
         <v>Thermal Curtain</v>
@@ -4405,10 +4405,10 @@
         <v>Light-Filtering Zebra Blinds</v>
       </c>
       <c r="C38" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D38" t="str">
-        <v>2f5bfaf3-39b1-4cba-9796-0a127d606c70</v>
+        <v>a3d63bbd-beea-4c82-829f-df9289344c60</v>
       </c>
       <c r="E38" t="str">
         <v>Noise Reducing Curtain</v>
@@ -4494,10 +4494,10 @@
         <v>Light-Filtering Zebra Blinds</v>
       </c>
       <c r="C39" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D39" t="str">
-        <v>2f5bfaf3-39b1-4cba-9796-0a127d606c70</v>
+        <v>a3d63bbd-beea-4c82-829f-df9289344c60</v>
       </c>
       <c r="E39" t="str">
         <v>Sheer White Curtain</v>
@@ -4583,10 +4583,10 @@
         <v>Light-Filtering Zebra Blinds</v>
       </c>
       <c r="C40" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D40" t="str">
-        <v>2f5bfaf3-39b1-4cba-9796-0a127d606c70</v>
+        <v>a3d63bbd-beea-4c82-829f-df9289344c60</v>
       </c>
       <c r="E40" t="str">
         <v>Patterned Curtain</v>
@@ -4672,10 +4672,10 @@
         <v>Light-Filtering Zebra Blinds</v>
       </c>
       <c r="C41" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D41" t="str">
-        <v>2f5bfaf3-39b1-4cba-9796-0a127d606c70</v>
+        <v>a3d63bbd-beea-4c82-829f-df9289344c60</v>
       </c>
       <c r="E41" t="str">
         <v>Kids Room Curtain</v>
@@ -4761,10 +4761,10 @@
         <v>Light-Filtering Zebra Blinds</v>
       </c>
       <c r="C42" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D42" t="str">
-        <v>2f5bfaf3-39b1-4cba-9796-0a127d606c70</v>
+        <v>a3d63bbd-beea-4c82-829f-df9289344c60</v>
       </c>
       <c r="E42" t="str">
         <v>Bedroom Blackout Curtain</v>
@@ -4850,10 +4850,10 @@
         <v>Light-Filtering Zebra Blinds</v>
       </c>
       <c r="C43" t="str">
-        <v>ac5f6482-6793-45d0-a65f-3b53c430d985</v>
+        <v>f81bc381-36e7-4364-940f-ec5aeac8cfdb</v>
       </c>
       <c r="D43" t="str">
-        <v>2f5bfaf3-39b1-4cba-9796-0a127d606c70</v>
+        <v>a3d63bbd-beea-4c82-829f-df9289344c60</v>
       </c>
       <c r="E43" t="str">
         <v>Living Room Curtain</v>
@@ -4939,10 +4939,10 @@
         <v>Blackout Vertical Blinds</v>
       </c>
       <c r="C44" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D44" t="str">
-        <v>373279f4-80e5-48c4-b051-a1c45ef22472</v>
+        <v>3807807b-b44a-4d4d-9bda-12646e61f6a3</v>
       </c>
       <c r="E44" t="str">
         <v>Window Valance</v>
@@ -5028,10 +5028,10 @@
         <v>Blackout Vertical Blinds</v>
       </c>
       <c r="C45" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D45" t="str">
-        <v>373279f4-80e5-48c4-b051-a1c45ef22472</v>
+        <v>3807807b-b44a-4d4d-9bda-12646e61f6a3</v>
       </c>
       <c r="E45" t="str">
         <v>Straight Valance</v>
@@ -5117,10 +5117,10 @@
         <v>Blackout Vertical Blinds</v>
       </c>
       <c r="C46" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D46" t="str">
-        <v>373279f4-80e5-48c4-b051-a1c45ef22472</v>
+        <v>3807807b-b44a-4d4d-9bda-12646e61f6a3</v>
       </c>
       <c r="E46" t="str">
         <v>Box Pleat Valance</v>
@@ -5206,10 +5206,10 @@
         <v>Blackout Vertical Blinds</v>
       </c>
       <c r="C47" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D47" t="str">
-        <v>373279f4-80e5-48c4-b051-a1c45ef22472</v>
+        <v>3807807b-b44a-4d4d-9bda-12646e61f6a3</v>
       </c>
       <c r="E47" t="str">
         <v>Decor Trim Valance</v>
@@ -5295,10 +5295,10 @@
         <v>Blackout Vertical Blinds</v>
       </c>
       <c r="C48" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D48" t="str">
-        <v>373279f4-80e5-48c4-b051-a1c45ef22472</v>
+        <v>3807807b-b44a-4d4d-9bda-12646e61f6a3</v>
       </c>
       <c r="E48" t="str">
         <v>Blind Mounting Kit</v>
@@ -5384,10 +5384,10 @@
         <v>Blackout Vertical Blinds</v>
       </c>
       <c r="C49" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D49" t="str">
-        <v>373279f4-80e5-48c4-b051-a1c45ef22472</v>
+        <v>3807807b-b44a-4d4d-9bda-12646e61f6a3</v>
       </c>
       <c r="E49" t="str">
         <v>Ceiling Mount Bracket</v>
@@ -5473,10 +5473,10 @@
         <v>Blackout Vertical Blinds</v>
       </c>
       <c r="C50" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D50" t="str">
-        <v>373279f4-80e5-48c4-b051-a1c45ef22472</v>
+        <v>3807807b-b44a-4d4d-9bda-12646e61f6a3</v>
       </c>
       <c r="E50" t="str">
         <v>Wall Mount Bracket</v>
@@ -5562,10 +5562,10 @@
         <v>Blackout Vertical Blinds</v>
       </c>
       <c r="C51" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D51" t="str">
-        <v>373279f4-80e5-48c4-b051-a1c45ef22472</v>
+        <v>3807807b-b44a-4d4d-9bda-12646e61f6a3</v>
       </c>
       <c r="E51" t="str">
         <v>Heavy Duty Bracket</v>
@@ -5651,10 +5651,10 @@
         <v>Blackout Vertical Blinds</v>
       </c>
       <c r="C52" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D52" t="str">
-        <v>373279f4-80e5-48c4-b051-a1c45ef22472</v>
+        <v>3807807b-b44a-4d4d-9bda-12646e61f6a3</v>
       </c>
       <c r="E52" t="str">
         <v>Slim Panel Blind</v>
@@ -5740,10 +5740,10 @@
         <v>Dimout Vertical Blinds</v>
       </c>
       <c r="C53" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D53" t="str">
-        <v>1d22baed-ba60-4747-b8aa-aece33843d86</v>
+        <v>437d4659-7f77-4f1c-be9b-5589924e665a</v>
       </c>
       <c r="E53" t="str">
         <v>Wide Panel Blind</v>
@@ -5829,10 +5829,10 @@
         <v>Dimout Vertical Blinds</v>
       </c>
       <c r="C54" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D54" t="str">
-        <v>1d22baed-ba60-4747-b8aa-aece33843d86</v>
+        <v>437d4659-7f77-4f1c-be9b-5589924e665a</v>
       </c>
       <c r="E54" t="str">
         <v>Honeycomb Cellular Shade</v>
@@ -5918,10 +5918,10 @@
         <v>Dimout Vertical Blinds</v>
       </c>
       <c r="C55" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D55" t="str">
-        <v>1d22baed-ba60-4747-b8aa-aece33843d86</v>
+        <v>437d4659-7f77-4f1c-be9b-5589924e665a</v>
       </c>
       <c r="E55" t="str">
         <v>Top Down Bottom Up Shade</v>
@@ -6007,10 +6007,10 @@
         <v>Dimout Vertical Blinds</v>
       </c>
       <c r="C56" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D56" t="str">
-        <v>1d22baed-ba60-4747-b8aa-aece33843d86</v>
+        <v>437d4659-7f77-4f1c-be9b-5589924e665a</v>
       </c>
       <c r="E56" t="str">
         <v>Energy Saving Shade</v>
@@ -6096,10 +6096,10 @@
         <v>Dimout Vertical Blinds</v>
       </c>
       <c r="C57" t="str">
-        <v>37693b8e-e314-4075-ae14-e5b367c1d0b0</v>
+        <v>d92f6e1b-42b8-4244-8534-a90569cf1a89</v>
       </c>
       <c r="D57" t="str">
-        <v>1d22baed-ba60-4747-b8aa-aece33843d86</v>
+        <v>437d4659-7f77-4f1c-be9b-5589924e665a</v>
       </c>
       <c r="E57" t="str">
         <v>Custom Size Window Blind</v>

</xml_diff>